<commit_message>
Stage Class & Cover Sheet
</commit_message>
<xml_diff>
--- a/res/Cover Sheet.xlsx
+++ b/res/Cover Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Cycling Coursework\ECM1410-Cycling-Coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C283765F-B715-4015-B075-81F3B0C516DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8DC065-A63A-416A-B34E-84A06088D5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FEDA237A-CB59-44E2-BB4C-2D01C6940287}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67172D40-6469-4B63-AC56-567EDFE716DF}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,10 +521,30 @@
       <c r="C9" s="2">
         <v>0.625</v>
       </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>45355</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited removeStageById by removing the checkpoints times and results from rider and removing it, edited removeCheckpoint
</commit_message>
<xml_diff>
--- a/res/Cover Sheet.xlsx
+++ b/res/Cover Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandy\source\repos\OOP Coursework\ECM1410-Cycling-Coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43532D9B-9E8E-4E3B-BE43-D512A7EB51AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A26287-4D04-4DE8-BCDF-583E60B7423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="348" yWindow="408" windowWidth="17280" windowHeight="8964" xr2:uid="{FEDA237A-CB59-44E2-BB4C-2D01C6940287}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Implementation Code</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Observer</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67172D40-6469-4B63-AC56-567EDFE716DF}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,6 +662,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>45370</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>45370</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edited Rider Result Deletion
</commit_message>
<xml_diff>
--- a/res/Cover Sheet.xlsx
+++ b/res/Cover Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Cycling Coursework\ECM1410-Cycling-Coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3EBE44-A619-42E4-8672-1F5B50A54C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F8F0AE-08CC-4872-B8F3-11FAAFA2C6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FEDA237A-CB59-44E2-BB4C-2D01C6940287}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>#Swapped Between Observer and Driver</t>
+  </si>
+  <si>
+    <t>#Swapping Between Observer and Driver</t>
+  </si>
+  <si>
+    <t>Observer/Driver</t>
   </si>
 </sst>
 </file>
@@ -110,11 +116,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67172D40-6469-4B63-AC56-567EDFE716DF}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>45370</v>
       </c>
@@ -685,7 +694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>45370</v>
       </c>
@@ -702,7 +711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>45373</v>
       </c>
@@ -719,7 +728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>45376</v>
       </c>
@@ -736,7 +745,44 @@
         <v>10</v>
       </c>
     </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>45376</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>45376</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A bit more testing code
</commit_message>
<xml_diff>
--- a/res/Cover Sheet.xlsx
+++ b/res/Cover Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Cycling Coursework\ECM1410-Cycling-Coursework\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandy\source\repos\OOP Coursework\ECM1410-Cycling-Coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F8F0AE-08CC-4872-B8F3-11FAAFA2C6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEDD3CE-8D5C-4E6F-B656-B7B84A63071D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FEDA237A-CB59-44E2-BB4C-2D01C6940287}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FEDA237A-CB59-44E2-BB4C-2D01C6940287}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -458,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67172D40-6469-4B63-AC56-567EDFE716DF}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,10 +730,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
-        <v>45376</v>
+        <v>45374</v>
       </c>
       <c r="C20" s="2">
-        <v>0.29166666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -747,41 +747,80 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
-        <v>45376</v>
+        <v>45375</v>
       </c>
       <c r="C21" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>45376</v>
       </c>
       <c r="C22" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="4"/>
     </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>45376</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>45376</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>